<commit_message>
Preliminary ZH support (not complete)
</commit_message>
<xml_diff>
--- a/Excel-DB/ConversationDB.xlsx
+++ b/Excel-DB/ConversationDB.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ian Meharg\Documents\Repositories\Web\lapin-cb\Excel-DB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{50D94A0D-542B-492A-8FF1-538FB63DF037}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD0CE694-0801-41AA-8395-9E0D6E02E8D0}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1500" yWindow="1380" windowWidth="15480" windowHeight="13965" xr2:uid="{E71A48F6-40D9-406C-AFE2-B445AE31C0AD}"/>
+    <workbookView xWindow="2940" yWindow="510" windowWidth="25185" windowHeight="13935" xr2:uid="{E71A48F6-40D9-406C-AFE2-B445AE31C0AD}"/>
   </bookViews>
   <sheets>
     <sheet name="Response Data" sheetId="1" r:id="rId1"/>
@@ -22,12 +22,13 @@
     <definedName name="DB_NAME">'Response Data'!$A$4</definedName>
     <definedName name="ORIGIN_ALIAS">Aliases!$A$3</definedName>
     <definedName name="ORIGIN_CONN">Connections!$A$2</definedName>
-    <definedName name="ORIGIN_DATA">'Response Data'!$A$7</definedName>
+    <definedName name="ORIGIN_DATA">'Response Data'!$A$9</definedName>
     <definedName name="ORIGIN_DEF">Defaults!$A$3</definedName>
+    <definedName name="PLACEHOLDER_1">'Response Data'!$B$6</definedName>
     <definedName name="STARTUP_MSG">'Response Data'!$F$4</definedName>
     <definedName name="WINDOW_TITLE">'Response Data'!#REF!</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -43,7 +44,31 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="144">
+  <si>
+    <t>よろしく</t>
+  </si>
+  <si>
+    <t>何日</t>
+  </si>
+  <si>
+    <t>あなた</t>
+  </si>
+  <si>
+    <t>名</t>
+  </si>
+  <si>
+    <t>貴方</t>
+  </si>
+  <si>
+    <t>君</t>
+  </si>
+  <si>
+    <t>お前</t>
+  </si>
+  <si>
+    <t>あんた</t>
+  </si>
   <si>
     <t>Default Conversational Database</t>
   </si>
@@ -69,6 +94,12 @@
     <t>Long Answer (first time)</t>
   </si>
   <si>
+    <t>よろしくね！</t>
+  </si>
+  <si>
+    <t>名前、ですか？私はただの回答スクリプトだから、ありませんね。</t>
+  </si>
+  <si>
     <t>Connection</t>
   </si>
   <si>
@@ -307,12 +338,39 @@
     <t>Notes</t>
   </si>
   <si>
+    <t>あなたの名前は？</t>
+  </si>
+  <si>
     <t>%okay%</t>
   </si>
   <si>
+    <t>分かりました！</t>
+  </si>
+  <si>
+    <t>OK！</t>
+  </si>
+  <si>
     <t>%what%</t>
   </si>
   <si>
+    <t>ごめん、エラーが起こっちゃったみたいです。</t>
+  </si>
+  <si>
+    <t>またエラーか…</t>
+  </si>
+  <si>
+    <t>うーん、正直に言って今のが分からなかったですね。簡単な質問にはお答えできます。</t>
+  </si>
+  <si>
+    <t>ごめん、質問が分かりません。</t>
+  </si>
+  <si>
+    <t>今</t>
+  </si>
+  <si>
+    <t>時間</t>
+  </si>
+  <si>
     <t>Original Keyword</t>
   </si>
   <si>
@@ -322,6 +380,30 @@
     <t>Words in this list will be converted before looking up an answer.</t>
   </si>
   <si>
+    <t>何時</t>
+  </si>
+  <si>
+    <t>何時に開きます？→時間に開きます？だが「時間」なら拾われます</t>
+  </si>
+  <si>
+    <t>なんじ</t>
+  </si>
+  <si>
+    <t>分からない</t>
+  </si>
+  <si>
+    <t>分かりません</t>
+  </si>
+  <si>
+    <t>わかりません</t>
+  </si>
+  <si>
+    <t>わかんない</t>
+  </si>
+  <si>
+    <t>いいですか</t>
+  </si>
+  <si>
     <t>Phrases in this list will appear in the "Default Selection" button menu that appears when a user indicates confusion.</t>
   </si>
   <si>
@@ -331,9 +413,33 @@
     <t>question-circle</t>
   </si>
   <si>
+    <t>質問に戻る</t>
+  </si>
+  <si>
+    <t>さようなら</t>
+  </si>
+  <si>
+    <t>またね！</t>
+  </si>
+  <si>
+    <t>分かりました！このチャットを閉じば再起動します。</t>
+  </si>
+  <si>
+    <t>また今度</t>
+  </si>
+  <si>
+    <t>またこんど</t>
+  </si>
+  <si>
+    <t>ありません</t>
+  </si>
+  <si>
     <t>X</t>
   </si>
   <si>
+    <t>また</t>
+  </si>
+  <si>
     <r>
       <rPr>
         <sz val="11"/>
@@ -498,12 +604,72 @@
     <t>X and only X</t>
   </si>
   <si>
+    <t>よくある選択肢を見てみよう。</t>
+  </si>
+  <si>
+    <t>いくつかおすすめの項目がありますが、いかがでしょうか？</t>
+  </si>
+  <si>
+    <t>わたし</t>
+  </si>
+  <si>
+    <t>私</t>
+  </si>
+  <si>
+    <t>俺</t>
+  </si>
+  <si>
+    <t>おれ</t>
+  </si>
+  <si>
+    <t>僕</t>
+  </si>
+  <si>
+    <t>ぼく</t>
+  </si>
+  <si>
+    <t>わたくし</t>
+  </si>
+  <si>
+    <t>ない。</t>
+  </si>
+  <si>
+    <t>は</t>
+  </si>
+  <si>
+    <t>THIS REQUIRES TESTING</t>
+  </si>
+  <si>
+    <t>私の名前は</t>
+  </si>
+  <si>
     <t>私は「」です</t>
   </si>
   <si>
+    <t>よろしくお願いします！</t>
+  </si>
+  <si>
     <t>Disables keywords other than that which came just before this connector.</t>
   </si>
   <si>
+    <t>名前</t>
+  </si>
+  <si>
+    <t>そうですか！ええと、質問があれば質問だけを送ってもらえば助かります。</t>
+  </si>
+  <si>
+    <t>そうですか…残念ながら私は記憶そのものがありませんけどね。</t>
+  </si>
+  <si>
+    <t>そうですか！初めまして。</t>
+  </si>
+  <si>
+    <t>ごめん、やっぱり私は質問に答えるという機能しかありません。</t>
+  </si>
+  <si>
+    <t>ありがとう、でも名前をもらったとしても私は記憶がありません。</t>
+  </si>
+  <si>
     <t>Database Abbreviation</t>
   </si>
   <si>
@@ -546,6 +712,9 @@
     <t>^{0}[。、….！!？?]*$</t>
   </si>
   <si>
+    <t>.</t>
+  </si>
+  <si>
     <t>Keywords are in order of response priority (row) and sequence (column). Use one period (.) to denote "anything".</t>
   </si>
   <si>
@@ -564,196 +733,70 @@
     <t>%defaults%</t>
   </si>
   <si>
-    <t>Hmm... Sorry, I can't figure out what you're asking about. I can answer simple questions.</t>
-  </si>
-  <si>
-    <t>Sorry, I don't understand the question.</t>
-  </si>
-  <si>
-    <t>Uh oh. Something's caused an error in this chat bot.</t>
-  </si>
-  <si>
-    <t>Another error...</t>
-  </si>
-  <si>
-    <t>Understood!</t>
-  </si>
-  <si>
-    <t>Okay!</t>
-  </si>
-  <si>
-    <t>Would you care to take a look at some recommended options?</t>
-  </si>
-  <si>
-    <t>Let's see some usual options.</t>
-  </si>
-  <si>
-    <t>hello</t>
-  </si>
-  <si>
-    <t>Hello.</t>
-  </si>
-  <si>
-    <t>Hi, there!</t>
-  </si>
-  <si>
-    <t>greetings</t>
-  </si>
-  <si>
-    <t xml:space="preserve">hi </t>
-  </si>
-  <si>
-    <t xml:space="preserve">hello </t>
-  </si>
-  <si>
-    <t>hey</t>
-  </si>
-  <si>
-    <t>you</t>
-  </si>
-  <si>
-    <t>name</t>
-  </si>
-  <si>
-    <t>I'm</t>
-  </si>
-  <si>
-    <t>I am</t>
-  </si>
-  <si>
-    <t>My name</t>
-  </si>
-  <si>
-    <t>current</t>
-  </si>
-  <si>
-    <t>time</t>
-  </si>
-  <si>
-    <t>date</t>
-  </si>
-  <si>
-    <t>today</t>
-  </si>
-  <si>
-    <t>It's good to meet you! Do you have any  specific questions?</t>
-  </si>
-  <si>
-    <t>Indeed... Unfortunately I lack much in the way of memory, but I'll try to answer any questions.</t>
-  </si>
-  <si>
-    <t>My name is</t>
-  </si>
-  <si>
-    <t>My name's</t>
-  </si>
-  <si>
-    <t>Do you have a name?</t>
-  </si>
-  <si>
-    <t>goodbye</t>
-  </si>
-  <si>
-    <t>good-bye</t>
-  </si>
-  <si>
-    <t>have a good day</t>
-  </si>
-  <si>
-    <t>have a nice day</t>
-  </si>
-  <si>
-    <t>nope</t>
-  </si>
-  <si>
-    <t>none</t>
-  </si>
-  <si>
-    <t>nice</t>
-  </si>
-  <si>
-    <t>fantastic</t>
-  </si>
-  <si>
-    <t>great</t>
-  </si>
-  <si>
-    <t>good</t>
-  </si>
-  <si>
-    <t>perfect</t>
-  </si>
-  <si>
-    <t>excellent</t>
-  </si>
-  <si>
-    <t>outstanding</t>
-  </si>
-  <si>
-    <t>love it</t>
-  </si>
-  <si>
-    <t>thanks</t>
-  </si>
-  <si>
-    <t>thank you</t>
-  </si>
-  <si>
-    <t>I don't know</t>
-  </si>
-  <si>
-    <t>dunno</t>
-  </si>
-  <si>
-    <t>I don't understand</t>
-  </si>
-  <si>
-    <t>what</t>
-  </si>
-  <si>
-    <t>listening</t>
-  </si>
-  <si>
-    <t>Resume</t>
-  </si>
-  <si>
-    <t>Name? Me? Whew, I'm not sophisticated enough for that.</t>
-  </si>
-  <si>
-    <t>I appreciate the gesture... Without any real memory, however, I don't need a name.</t>
-  </si>
-  <si>
-    <t>Until we meet again!</t>
-  </si>
-  <si>
-    <t>Goodbye! You can close this chat to restart it.</t>
-  </si>
-  <si>
-    <t>Okay! You can close this chat to restart it.</t>
-  </si>
-  <si>
-    <t>later</t>
-  </si>
-  <si>
-    <t>I'm glad you're pleased.</t>
-  </si>
-  <si>
-    <t>Isn't it?</t>
-  </si>
-  <si>
-    <t>glad</t>
-  </si>
-  <si>
-    <t>Good to hear.</t>
-  </si>
-  <si>
-    <t>Great!</t>
-  </si>
-  <si>
-    <t>You're quite welcome.</t>
-  </si>
-  <si>
-    <t>You're welcome.</t>
+    <t>いいね</t>
+  </si>
+  <si>
+    <t>いえいえ。ありがとうございます。</t>
+  </si>
+  <si>
+    <t>すみません、ありがとうございます。</t>
+  </si>
+  <si>
+    <t>すばらしい</t>
+  </si>
+  <si>
+    <t>素晴らしい</t>
+  </si>
+  <si>
+    <t>すごい</t>
+  </si>
+  <si>
+    <t>スゴイ</t>
+  </si>
+  <si>
+    <t>完璧</t>
+  </si>
+  <si>
+    <t>よかった</t>
+  </si>
+  <si>
+    <t>恐縮です。</t>
+  </si>
+  <si>
+    <t>良いね</t>
+  </si>
+  <si>
+    <t>ナイス</t>
+  </si>
+  <si>
+    <t>ありがとう</t>
+  </si>
+  <si>
+    <t>どういたしまして。</t>
+  </si>
+  <si>
+    <t>いえいえ。</t>
+  </si>
+  <si>
+    <t>アリガトウ</t>
+  </si>
+  <si>
+    <t>有難う</t>
+  </si>
+  <si>
+    <t>Text placeholder</t>
+  </si>
+  <si>
+    <t>First time</t>
+  </si>
+  <si>
+    <t>Afterwards</t>
+  </si>
+  <si>
+    <t>...</t>
+  </si>
+  <si>
+    <t>ここで質問を記入してください</t>
   </si>
 </sst>
 </file>
@@ -1201,10 +1244,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78C711C4-F497-477F-BE97-0DB07361B6EC}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:I102"/>
+  <dimension ref="A1:I105"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5:XFD6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1219,317 +1262,357 @@
   <sheetData>
     <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="F1" s="4"/>
       <c r="G1" s="4"/>
     </row>
     <row r="2" spans="1:9" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="B2" s="2"/>
     </row>
     <row r="3" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
-        <v>46</v>
+        <v>101</v>
       </c>
       <c r="F3" s="12"/>
       <c r="G3" s="12"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="F5" s="4"/>
-      <c r="G5" s="4"/>
-    </row>
-    <row r="6" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B6" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D6" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F6" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="G6" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="H6" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="I6" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>27</v>
-      </c>
-      <c r="F7" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="G7" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="H7" s="3"/>
-    </row>
-    <row r="8" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>2</v>
-      </c>
-      <c r="F8" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="G8" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="H8" s="3"/>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="10" t="s">
+        <v>139</v>
+      </c>
+      <c r="B5" s="10" t="s">
+        <v>140</v>
+      </c>
+      <c r="D5" s="10" t="s">
+        <v>141</v>
+      </c>
+      <c r="F5" s="12"/>
+      <c r="G5" s="12"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>143</v>
+      </c>
+      <c r="D6" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="F7" s="4"/>
+      <c r="G7" s="4"/>
+    </row>
+    <row r="8" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D8" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G8" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>26</v>
+        <v>40</v>
       </c>
       <c r="F9" s="6" t="s">
-        <v>70</v>
+        <v>43</v>
       </c>
       <c r="G9" s="6" t="s">
-        <v>71</v>
+        <v>44</v>
       </c>
       <c r="H9" s="3"/>
     </row>
     <row r="10" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>65</v>
+        <v>10</v>
       </c>
       <c r="F10" s="6" t="s">
-        <v>72</v>
+        <v>41</v>
       </c>
       <c r="G10" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="H10" s="3" t="s">
-        <v>64</v>
-      </c>
+        <v>42</v>
+      </c>
+      <c r="H10" s="3"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>74</v>
+        <v>37</v>
       </c>
       <c r="F11" s="6" t="s">
-        <v>76</v>
+        <v>38</v>
       </c>
       <c r="G11" s="6" t="s">
-        <v>75</v>
+        <v>39</v>
       </c>
       <c r="H11" s="3"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>86</v>
-      </c>
-      <c r="B12" t="s">
-        <v>10</v>
-      </c>
-      <c r="C12" t="s">
-        <v>87</v>
-      </c>
-      <c r="F12" s="6"/>
-      <c r="G12" s="6"/>
+        <v>121</v>
+      </c>
+      <c r="F12" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="G12" s="6" t="s">
+        <v>79</v>
+      </c>
       <c r="H12" s="3" t="s">
-        <v>62</v>
+        <v>120</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>88</v>
-      </c>
-      <c r="B13" t="s">
-        <v>10</v>
-      </c>
-      <c r="C13" t="s">
+        <v>0</v>
+      </c>
+      <c r="F13" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="G13" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="H13" s="3"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>45</v>
+      </c>
+      <c r="B14" t="s">
+        <v>20</v>
+      </c>
+      <c r="C14" t="s">
+        <v>46</v>
+      </c>
+      <c r="F14" s="6"/>
+      <c r="G14" s="6"/>
+      <c r="H14" s="3" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>1</v>
+      </c>
+      <c r="F15" s="6"/>
+      <c r="G15" s="6"/>
+      <c r="H15" s="3" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>81</v>
+      </c>
+      <c r="B16" t="s">
+        <v>19</v>
+      </c>
+      <c r="C16" t="s">
         <v>89</v>
       </c>
-      <c r="F13" s="6"/>
-      <c r="G13" s="6"/>
-      <c r="H13" s="3" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>84</v>
-      </c>
-      <c r="F14" s="6" t="s">
-        <v>90</v>
-      </c>
-      <c r="G14" s="6" t="s">
-        <v>91</v>
-      </c>
-      <c r="H14" s="3"/>
-      <c r="I14" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>81</v>
-      </c>
-      <c r="B15" t="s">
-        <v>11</v>
-      </c>
-      <c r="C15" t="s">
-        <v>82</v>
-      </c>
-      <c r="F15" s="6" t="s">
-        <v>117</v>
-      </c>
-      <c r="G15" s="6" t="s">
-        <v>118</v>
-      </c>
-      <c r="H15" s="3"/>
-      <c r="I15" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>95</v>
+      <c r="D16" t="s">
+        <v>21</v>
+      </c>
+      <c r="E16" t="s">
+        <v>115</v>
       </c>
       <c r="F16" s="6" t="s">
-        <v>120</v>
+        <v>96</v>
       </c>
       <c r="G16" s="6" t="s">
-        <v>119</v>
-      </c>
-      <c r="H16" s="11"/>
-    </row>
-    <row r="17" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+        <v>97</v>
+      </c>
+      <c r="H16" s="3"/>
+      <c r="I16" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>81</v>
       </c>
       <c r="B17" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="C17" t="s">
+        <v>3</v>
+      </c>
+      <c r="D17" t="s">
+        <v>19</v>
+      </c>
+      <c r="E17" t="s">
+        <v>89</v>
+      </c>
+      <c r="F17" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="G17" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="H17" s="3"/>
+      <c r="I17" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>2</v>
+      </c>
+      <c r="B18" t="s">
+        <v>20</v>
+      </c>
+      <c r="C18" t="s">
+        <v>3</v>
+      </c>
+      <c r="F18" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="G18" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="H18" s="3"/>
+      <c r="I18" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>62</v>
+      </c>
+      <c r="F19" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="G19" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="H19" s="11"/>
+    </row>
+    <row r="20" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>69</v>
+      </c>
+      <c r="B20" t="s">
+        <v>71</v>
+      </c>
+      <c r="C20" t="s">
+        <v>89</v>
+      </c>
+      <c r="F20" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="G20" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="H20" s="11"/>
+      <c r="I20" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
         <v>122</v>
       </c>
-      <c r="F17" s="6" t="s">
-        <v>121</v>
-      </c>
-      <c r="G17" s="6" t="s">
-        <v>119</v>
-      </c>
-      <c r="H17" s="11"/>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>101</v>
-      </c>
-      <c r="F18" s="6" t="s">
+      <c r="F21" s="6" t="s">
         <v>123</v>
       </c>
-      <c r="G18" s="6" t="s">
+      <c r="G21" s="6" t="s">
         <v>124</v>
       </c>
-      <c r="H18" s="3"/>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>125</v>
-      </c>
-      <c r="F19" s="6" t="s">
-        <v>127</v>
-      </c>
-      <c r="G19" s="6" t="s">
-        <v>126</v>
-      </c>
-      <c r="H19" s="3"/>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>109</v>
-      </c>
-      <c r="F20" s="6" t="s">
-        <v>128</v>
-      </c>
-      <c r="G20" s="6" t="s">
-        <v>129</v>
-      </c>
-      <c r="H20" s="3"/>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="F21" s="6"/>
-      <c r="G21" s="6"/>
       <c r="H21" s="3"/>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="F22" s="6"/>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>130</v>
+      </c>
+      <c r="F22" s="6" t="s">
+        <v>131</v>
+      </c>
       <c r="G22" s="6"/>
       <c r="H22" s="3"/>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="F23" s="6"/>
-      <c r="G23" s="6"/>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>134</v>
+      </c>
+      <c r="F23" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="G23" s="6" t="s">
+        <v>136</v>
+      </c>
       <c r="H23" s="3"/>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F24" s="6"/>
       <c r="G24" s="6"/>
       <c r="H24" s="3"/>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F25" s="6"/>
       <c r="G25" s="6"/>
       <c r="H25" s="3"/>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F26" s="6"/>
       <c r="G26" s="6"/>
       <c r="H26" s="3"/>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F27" s="6"/>
       <c r="G27" s="6"/>
       <c r="H27" s="3"/>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F28" s="6"/>
       <c r="G28" s="6"/>
       <c r="H28" s="3"/>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="F29" s="7"/>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F29" s="6"/>
       <c r="G29" s="6"/>
       <c r="H29" s="3"/>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="F30" s="7"/>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F30" s="6"/>
       <c r="G30" s="6"/>
       <c r="H30" s="3"/>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="F31" s="7"/>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F31" s="6"/>
       <c r="G31" s="6"/>
       <c r="H31" s="3"/>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F32" s="7"/>
       <c r="G32" s="6"/>
       <c r="H32" s="3"/>
@@ -1883,6 +1966,21 @@
       <c r="F102" s="7"/>
       <c r="G102" s="6"/>
       <c r="H102" s="3"/>
+    </row>
+    <row r="103" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F103" s="7"/>
+      <c r="G103" s="6"/>
+      <c r="H103" s="3"/>
+    </row>
+    <row r="104" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F104" s="7"/>
+      <c r="G104" s="6"/>
+      <c r="H104" s="3"/>
+    </row>
+    <row r="105" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F105" s="7"/>
+      <c r="G105" s="6"/>
+      <c r="H105" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1894,7 +1992,7 @@
           <x14:formula1>
             <xm:f>Connections!$A$2:$A$10</xm:f>
           </x14:formula1>
-          <xm:sqref>B7:B17 D7:D17</xm:sqref>
+          <xm:sqref>D9:D20 B9:B20</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -1920,29 +2018,29 @@
   <sheetData>
     <row r="1" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
-        <v>31</v>
+        <v>58</v>
       </c>
     </row>
     <row r="2" spans="1:3" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
-        <v>48</v>
+        <v>103</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>49</v>
+        <v>104</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>32</v>
+        <v>59</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>116</v>
+        <v>61</v>
       </c>
       <c r="B3" t="s">
-        <v>26</v>
+        <v>37</v>
       </c>
       <c r="C3" t="s">
-        <v>33</v>
+        <v>60</v>
       </c>
     </row>
   </sheetData>
@@ -1953,10 +2051,10 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7DB7BD8A-D265-46FE-8A2B-63E63510F07C}">
   <sheetPr codeName="Sheet3"/>
-  <dimension ref="A1:C27"/>
+  <dimension ref="A1:C33"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1967,218 +2065,269 @@
   <sheetData>
     <row r="1" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
-        <v>30</v>
+        <v>49</v>
       </c>
     </row>
     <row r="2" spans="1:3" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
-        <v>29</v>
+        <v>48</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>28</v>
+        <v>47</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>25</v>
+        <v>35</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>77</v>
+        <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>74</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>78</v>
+        <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>79</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>80</v>
+        <v>6</v>
       </c>
       <c r="B5" t="s">
-        <v>74</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>83</v>
+        <v>7</v>
       </c>
       <c r="B6" t="s">
-        <v>84</v>
+        <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="B7" t="s">
-        <v>84</v>
+        <v>3</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>93</v>
+        <v>50</v>
       </c>
       <c r="B8" t="s">
-        <v>84</v>
+        <v>46</v>
+      </c>
+      <c r="C8" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>85</v>
+        <v>52</v>
       </c>
       <c r="B9" t="s">
-        <v>84</v>
+        <v>46</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>111</v>
+        <v>53</v>
       </c>
       <c r="B10" t="s">
-        <v>65</v>
+        <v>121</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>112</v>
+        <v>54</v>
       </c>
       <c r="B11" t="s">
-        <v>65</v>
+        <v>121</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>113</v>
+        <v>55</v>
       </c>
       <c r="B12" t="s">
-        <v>65</v>
+        <v>121</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>114</v>
+        <v>56</v>
       </c>
       <c r="B13" t="s">
-        <v>65</v>
+        <v>121</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>115</v>
+        <v>57</v>
       </c>
       <c r="B14" t="s">
-        <v>26</v>
+        <v>37</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>96</v>
+        <v>65</v>
       </c>
       <c r="B15" t="s">
-        <v>95</v>
+        <v>62</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>97</v>
+        <v>66</v>
       </c>
       <c r="B16" t="s">
-        <v>95</v>
+        <v>62</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>98</v>
+        <v>88</v>
       </c>
       <c r="B17" t="s">
-        <v>95</v>
+        <v>62</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>99</v>
+        <v>67</v>
       </c>
       <c r="B18" t="s">
-        <v>95</v>
+        <v>62</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>100</v>
+        <v>87</v>
       </c>
       <c r="B19" t="s">
-        <v>95</v>
+        <v>81</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>102</v>
+        <v>82</v>
       </c>
       <c r="B20" t="s">
-        <v>101</v>
+        <v>81</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>103</v>
+        <v>83</v>
       </c>
       <c r="B21" t="s">
-        <v>101</v>
+        <v>81</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>104</v>
+        <v>84</v>
       </c>
       <c r="B22" t="s">
-        <v>101</v>
+        <v>81</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>105</v>
+        <v>85</v>
       </c>
       <c r="B23" t="s">
-        <v>101</v>
+        <v>81</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>106</v>
+        <v>86</v>
       </c>
       <c r="B24" t="s">
-        <v>101</v>
+        <v>81</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>107</v>
+        <v>125</v>
       </c>
       <c r="B25" t="s">
-        <v>101</v>
+        <v>122</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>108</v>
+        <v>126</v>
       </c>
       <c r="B26" t="s">
-        <v>101</v>
+        <v>122</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>110</v>
+        <v>127</v>
       </c>
       <c r="B27" t="s">
-        <v>109</v>
+        <v>122</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>128</v>
+      </c>
+      <c r="B28" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>129</v>
+      </c>
+      <c r="B29" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>132</v>
+      </c>
+      <c r="B30" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>133</v>
+      </c>
+      <c r="B31" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>137</v>
+      </c>
+      <c r="B32" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>138</v>
+      </c>
+      <c r="B33" t="s">
+        <v>134</v>
       </c>
     </row>
   </sheetData>
@@ -2203,133 +2352,133 @@
   <sheetData>
     <row r="1" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>50</v>
+        <v>105</v>
       </c>
       <c r="C1" s="10" t="s">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="D1" s="10" t="s">
-        <v>14</v>
+        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C2" t="s">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="D2" t="s">
-        <v>24</v>
+        <v>34</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="B3" t="s">
-        <v>51</v>
+        <v>106</v>
       </c>
       <c r="C3" t="s">
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="D3" t="s">
-        <v>35</v>
+        <v>70</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="B4" t="s">
-        <v>52</v>
+        <v>107</v>
       </c>
       <c r="C4" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="D4" t="s">
-        <v>22</v>
+        <v>32</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="B5" t="s">
-        <v>53</v>
+        <v>108</v>
       </c>
       <c r="C5" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="D5" t="s">
-        <v>18</v>
+        <v>28</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>19</v>
+        <v>29</v>
       </c>
       <c r="B6" t="s">
-        <v>54</v>
+        <v>109</v>
       </c>
       <c r="C6" t="s">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="D6" t="s">
-        <v>21</v>
+        <v>31</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>36</v>
+        <v>71</v>
       </c>
       <c r="B7" t="s">
-        <v>55</v>
+        <v>110</v>
       </c>
       <c r="C7" t="s">
-        <v>37</v>
+        <v>72</v>
       </c>
       <c r="D7" t="s">
-        <v>38</v>
+        <v>73</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>39</v>
+        <v>74</v>
       </c>
       <c r="B8" t="s">
-        <v>56</v>
+        <v>111</v>
       </c>
       <c r="C8" t="s">
-        <v>41</v>
+        <v>76</v>
       </c>
       <c r="D8" t="s">
-        <v>42</v>
+        <v>77</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>40</v>
+        <v>75</v>
       </c>
       <c r="B9" t="s">
-        <v>57</v>
+        <v>112</v>
       </c>
       <c r="C9" t="s">
-        <v>58</v>
+        <v>113</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>34</v>
+        <v>68</v>
       </c>
       <c r="B10" t="s">
-        <v>59</v>
+        <v>114</v>
       </c>
       <c r="C10" t="s">
-        <v>43</v>
+        <v>78</v>
       </c>
       <c r="D10" t="s">
-        <v>45</v>
+        <v>94</v>
       </c>
     </row>
   </sheetData>

</xml_diff>